<commit_message>
Updated Excel schema and the models.py file with new booleans in the Mission table
</commit_message>
<xml_diff>
--- a/smdb/docs/original/DatabaseSchema.xlsx
+++ b/smdb/docs/original/DatabaseSchema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paje/Documents/JennyMBARI/MappingDB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paje/Documents/JennyMBARI/SMDB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892EC810-1E76-5A47-ABAA-325053EED631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633205EF-8E4B-F047-9B00-AC072923D5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="460" windowWidth="50240" windowHeight="31540" xr2:uid="{9FFA2DA2-8C6E-0449-9A10-C54CFC4AB1E7}"/>
+    <workbookView xWindow="-44680" yWindow="-6620" windowWidth="41440" windowHeight="27300" xr2:uid="{9FFA2DA2-8C6E-0449-9A10-C54CFC4AB1E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$O$57</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="119">
   <si>
     <t>id</t>
   </si>
@@ -233,9 +233,6 @@
     <t>MissionType</t>
   </si>
   <si>
-    <t>(e.g., AUV mapping, LASS survey)</t>
-  </si>
-  <si>
     <t>Platform</t>
   </si>
   <si>
@@ -567,6 +564,21 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>serial_number</t>
+  </si>
+  <si>
+    <t>(e.g., years in use?</t>
+  </si>
+  <si>
+    <t>(e.g., AUV mapping, LASS, ship-based, iceberg_config)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD: series of status yes/no fields: testing, failed, dont_use, use_with_caution </t>
+  </si>
+  <si>
+    <t>patch_test</t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1081,8 @@
   </sheetPr>
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,24 +1097,24 @@
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" customWidth="1"/>
     <col min="10" max="10" width="22.5" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" customWidth="1"/>
     <col min="13" max="13" width="13.83203125" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -1114,28 +1126,28 @@
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>1</v>
@@ -1146,108 +1158,108 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
         <v>67</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>68</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" t="s">
         <v>112</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
@@ -1255,7 +1267,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I18" s="12"/>
     </row>
@@ -1265,370 +1277,388 @@
         <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J20" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I23" s="12"/>
       <c r="K23" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M23" s="12"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
         <v>105</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="G30" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L30" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M30" s="12"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="3" t="s">
         <v>0</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>32</v>
-      </c>
       <c r="G34" t="s">
-        <v>80</v>
-      </c>
-      <c r="K34" s="5"/>
-      <c r="L34" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="M34" s="7" t="s">
-        <v>25</v>
+        <v>79</v>
+      </c>
+      <c r="K34" s="2"/>
+      <c r="L34" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>29</v>
-      </c>
-      <c r="K35" t="s">
-        <v>111</v>
+      <c r="K35" s="5"/>
+      <c r="L35" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N35" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="K36" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
       <c r="B38" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>118</v>
+      </c>
       <c r="H41" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I41" s="11"/>
       <c r="J41" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -1637,62 +1667,62 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M42" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N42" s="12"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H43" s="2"/>
       <c r="I43" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L43" s="2"/>
       <c r="M43" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H44" s="5"/>
       <c r="I44" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C45" s="12"/>
       <c r="L45" s="2"/>
       <c r="M45" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -1701,185 +1731,185 @@
         <v>0</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N46" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
         <v>70</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
         <v>72</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>73</v>
-      </c>
       <c r="H48" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I48" s="11"/>
       <c r="J48" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="3" t="s">
         <v>0</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M49" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N49" s="12"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
         <v>75</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" t="s">
-        <v>76</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L50" s="2"/>
       <c r="M50" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L51" s="2"/>
       <c r="M51" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" t="s">
         <v>105</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" t="s">
-        <v>106</v>
       </c>
       <c r="L52" s="2"/>
       <c r="M52" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L53" s="5"/>
       <c r="M53" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N53" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
         <v>44</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>